<commit_message>
added payment logic for PD Course Booking edited Common Metadata with new course URL
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BC745B-9D4D-4765-AC49-516C056F97C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0B59CC-3083-49AD-BA08-34C7340B8DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -370,9 +370,6 @@
     <t>PDCOURSEURL</t>
   </si>
   <si>
-    <t>http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1</t>
-  </si>
-  <si>
     <t>CUSTOMERGROUP</t>
   </si>
   <si>
@@ -470,6 +467,9 @@
   </si>
   <si>
     <t>casemail777@yahoo.com</t>
+  </si>
+  <si>
+    <t>http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/automation-regression-course-do-not-amend</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -620,6 +619,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гіперпосилання" xfId="1" builtinId="8"/>
@@ -898,7 +898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -947,7 +947,7 @@
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -1286,10 +1286,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>5</v>
@@ -1297,32 +1297,32 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>142</v>
+        <v>139</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="26" t="s">
+      <c r="B38" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>147</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>5</v>
@@ -1460,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
@@ -1696,20 +1696,20 @@
         <v>114</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="B22" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="C22" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1724,19 +1724,18 @@
     <hyperlink ref="B14" r:id="rId7" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=jersey" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
     <hyperlink ref="B10" r:id="rId8" tooltip="https://web-stage-bppdigital.bppuniversity.com/account?registration_type=rbs" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
     <hyperlink ref="B20" r:id="rId9" tooltip="https://totara-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="B21" r:id="rId10" tooltip="http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/oksana-adm-course-1" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="B16" r:id="rId11" tooltip="https://web-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="B17" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="B15" r:id="rId13" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="B19" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="B11" r:id="rId15" tooltip="https://web-stage-bppdigital.bppuniversity.com/account" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink ref="B12" r:id="rId16" tooltip="https://admin-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink ref="B8" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="B9" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink ref="B22" r:id="rId19" xr:uid="{9A4B1622-C4FB-4D19-AD75-0B584A49AF59}"/>
+    <hyperlink ref="B16" r:id="rId10" tooltip="https://web-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="B17" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId12" tooltip="https://web-stage-bppdigital.bppuniversity.com/insights" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="B19" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="B11" r:id="rId14" tooltip="https://web-stage-bppdigital.bppuniversity.com/account" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="B12" r:id="rId15" tooltip="https://admin-stage-bppdigital.bppuniversity.com" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="B8" r:id="rId16" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="B9" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="B22" r:id="rId18" xr:uid="{9A4B1622-C4FB-4D19-AD75-0B584A49AF59}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -1768,10 +1767,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1779,10 +1778,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1790,7 +1789,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="2">
         <v>598587</v>
@@ -1801,10 +1800,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -1812,10 +1811,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -1823,10 +1822,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
@@ -1834,10 +1833,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -1845,10 +1844,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>5</v>
@@ -1856,10 +1855,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -1867,10 +1866,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
@@ -1878,10 +1877,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -1889,10 +1888,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>5</v>
@@ -1900,7 +1899,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" s="5">
         <v>10</v>
@@ -1911,7 +1910,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15" s="5">
         <v>2022</v>
@@ -1922,7 +1921,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B16" s="5">
         <v>737</v>

</xml_diff>

<commit_message>
created first test for eCommerce amended Metadata added 2 new SpecialStepDefs updated token for BE
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0B59CC-3083-49AD-BA08-34C7340B8DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62556561-C08E-438C-900A-772F0DEE8214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="153">
   <si>
     <t>Tag</t>
   </si>
@@ -470,13 +470,25 @@
   </si>
   <si>
     <t>http://web-stage-bppdigital.bppuniversity.com/courses/accountancy-and-tax/automation-regression-course-do-not-amend</t>
+  </si>
+  <si>
+    <t>BPPDIGITALECOMMERCEURL</t>
+  </si>
+  <si>
+    <t>http://web-stage-bppdigital.bppuniversity.com/ecommerceregression</t>
+  </si>
+  <si>
+    <t>VISACARDCVV</t>
+  </si>
+  <si>
+    <t>MASTERCARDNUMBER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +538,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -548,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,6 +639,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гіперпосилання" xfId="1" builtinId="8"/>
@@ -1458,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
@@ -1710,6 +1738,17 @@
         <v>143</v>
       </c>
       <c r="C22" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1733,18 +1772,19 @@
     <hyperlink ref="B8" r:id="rId16" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
     <hyperlink ref="B9" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
     <hyperlink ref="B22" r:id="rId18" xr:uid="{9A4B1622-C4FB-4D19-AD75-0B584A49AF59}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{44E35DEF-3D82-4C68-A685-583D7C6137E1}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
@@ -1930,7 +1970,30 @@
         <v>5</v>
       </c>
     </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="5">
+        <v>123</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="29">
+        <v>5555444433331110</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created new test for eCommerce Logged User refactored existing
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62556561-C08E-438C-900A-772F0DEE8214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D7ACDF-8619-49DF-9436-757800B35C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="156">
   <si>
     <t>Tag</t>
   </si>
@@ -482,6 +482,15 @@
   </si>
   <si>
     <t>MASTERCARDNUMBER</t>
+  </si>
+  <si>
+    <t>BPPDIGITALECOMMERCETWOURL</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/ecommerceregressionsecond</t>
+  </si>
+  <si>
+    <t>2222 4200 0000 1113</t>
   </si>
 </sst>
 </file>
@@ -1486,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
@@ -1749,6 +1758,17 @@
         <v>150</v>
       </c>
       <c r="C23" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1773,9 +1793,10 @@
     <hyperlink ref="B9" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
     <hyperlink ref="B22" r:id="rId18" xr:uid="{9A4B1622-C4FB-4D19-AD75-0B584A49AF59}"/>
     <hyperlink ref="B23" r:id="rId19" xr:uid="{44E35DEF-3D82-4C68-A685-583D7C6137E1}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{7472DB20-9DEC-4C20-BD8B-D306A19B4897}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -1784,7 +1805,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
@@ -1985,8 +2006,8 @@
       <c r="A18" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B18" s="29">
-        <v>5555444433331110</v>
+      <c r="B18" s="29" t="s">
+        <v>155</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
created new test for eCommerce Amex Card updated Metadata and token
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D7ACDF-8619-49DF-9436-757800B35C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB02E663-D25C-4B0E-ACE3-EE1C592DFCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="159">
   <si>
     <t>Tag</t>
   </si>
@@ -491,6 +491,15 @@
   </si>
   <si>
     <t>2222 4200 0000 1113</t>
+  </si>
+  <si>
+    <t>AMEXCARDNUMBER</t>
+  </si>
+  <si>
+    <t>3782 8224 6310 005</t>
+  </si>
+  <si>
+    <t>AMEXCARDCVV</t>
   </si>
 </sst>
 </file>
@@ -1802,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
@@ -2013,6 +2022,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="29">
+        <v>1234</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
refactored Case Management and Single Bookings tests due to latest changes updated tokens rolled back i_should_see_the_text() because SUM wasn't calculated correctly added new test for Ecommerce
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB02E663-D25C-4B0E-ACE3-EE1C592DFCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD5A92C-6EC5-4827-ABE5-FCBF18ACC4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="161">
   <si>
     <t>Tag</t>
   </si>
@@ -500,6 +500,12 @@
   </si>
   <si>
     <t>AMEXCARDCVV</t>
+  </si>
+  <si>
+    <t>BPPDIGITALECOMMERCELOCALSTORAGE</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/localstorage</t>
   </si>
 </sst>
 </file>
@@ -1504,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
@@ -1778,6 +1784,17 @@
         <v>154</v>
       </c>
       <c r="C24" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1803,9 +1820,10 @@
     <hyperlink ref="B22" r:id="rId18" xr:uid="{9A4B1622-C4FB-4D19-AD75-0B584A49AF59}"/>
     <hyperlink ref="B23" r:id="rId19" xr:uid="{44E35DEF-3D82-4C68-A685-583D7C6137E1}"/>
     <hyperlink ref="B24" r:id="rId20" xr:uid="{7472DB20-9DEC-4C20-BD8B-D306A19B4897}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{490AA195-2BCD-46BA-A815-E8816723E15C}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -1813,7 +1831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added Verification of papers and Bodies to eCommerce journey; amended Line Managers tests with Guerillamail services; updated token for Venus
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD5A92C-6EC5-4827-ABE5-FCBF18ACC4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBEBE2E-F492-4D16-8675-A1A210C63FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="163">
   <si>
     <t>Tag</t>
   </si>
@@ -506,18 +506,31 @@
   </si>
   <si>
     <t>https://web-stage-bppdigital.bppuniversity.com/localstorage</t>
+  </si>
+  <si>
+    <t>https://uat-products.bpp.com/courses/edit/07846e8a-20b6-425c-afa9-0bba2e6c7952</t>
+  </si>
+  <si>
+    <t>PRODUCTFACTORYUPDATEINSTANCEURL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -589,11 +602,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -606,70 +619,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1510,15 +1526,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
     <col min="2" max="2" width="140.44140625" customWidth="1"/>
     <col min="3" max="3" width="26.109375" customWidth="1"/>
   </cols>
@@ -1795,6 +1811,17 @@
         <v>160</v>
       </c>
       <c r="C25" s="17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1821,9 +1848,10 @@
     <hyperlink ref="B23" r:id="rId19" xr:uid="{44E35DEF-3D82-4C68-A685-583D7C6137E1}"/>
     <hyperlink ref="B24" r:id="rId20" xr:uid="{7472DB20-9DEC-4C20-BD8B-D306A19B4897}"/>
     <hyperlink ref="B25" r:id="rId21" xr:uid="{490AA195-2BCD-46BA-A815-E8816723E15C}"/>
+    <hyperlink ref="B26" r:id="rId22" xr:uid="{A2875131-586F-4E26-BAFD-7D53FBEA4B92}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Created test for Deactivation of Instance (will be completed after deploying https://jira.bpp.com/browse/BPP-18057 to UAT)
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBEBE2E-F492-4D16-8675-A1A210C63FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2346BEDB-0014-4663-BBA6-DBE77BCD6EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="165">
   <si>
     <t>Tag</t>
   </si>
@@ -512,13 +512,19 @@
   </si>
   <si>
     <t>PRODUCTFACTORYUPDATEINSTANCEURL</t>
+  </si>
+  <si>
+    <t>BPPDIGITALECOMMERCEDEACTIVATEURL</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/deactivateinstance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,13 +555,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -602,9 +601,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -619,42 +618,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -666,24 +643,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -966,16 +959,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.55"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" style="15" customWidth="1"/>
-    <col min="2" max="2" width="45.44140625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="44.109375" style="15" customWidth="1"/>
-    <col min="4" max="16384" width="8.6640625" style="15"/>
+    <col min="1" max="1" width="33.88671875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="45.44140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="8.6640625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
@@ -990,365 +983,365 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="8" customFormat="1">
-      <c r="A4" s="8" t="s">
+      <c r="C3" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="6" customFormat="1">
+      <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="8" customFormat="1">
-      <c r="A5" s="8" t="s">
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="6" customFormat="1">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="8" customFormat="1">
-      <c r="A6" s="8" t="s">
+      <c r="C5" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="6" customFormat="1">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="8" customFormat="1">
-      <c r="A7" s="8" t="s">
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="6" customFormat="1">
+      <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1367,7 +1360,7 @@
       <c r="A36" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="15" t="s">
         <v>141</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1375,24 +1368,24 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1445,7 +1438,7 @@
       <c r="A2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="11" t="s">
         <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1526,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
@@ -1551,10 +1544,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="22" t="s">
         <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1562,10 +1555,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="22" t="s">
         <v>80</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1573,10 +1566,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="22" t="s">
         <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1584,244 +1577,255 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1849,9 +1853,10 @@
     <hyperlink ref="B24" r:id="rId20" xr:uid="{7472DB20-9DEC-4C20-BD8B-D306A19B4897}"/>
     <hyperlink ref="B25" r:id="rId21" xr:uid="{490AA195-2BCD-46BA-A815-E8816723E15C}"/>
     <hyperlink ref="B26" r:id="rId22" xr:uid="{A2875131-586F-4E26-BAFD-7D53FBEA4B92}"/>
+    <hyperlink ref="B27" r:id="rId23" xr:uid="{7528A15C-B863-45DE-89E2-AF2401542240}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId23"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 
@@ -2061,7 +2066,7 @@
       <c r="A18" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="20" t="s">
         <v>155</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -2072,7 +2077,7 @@
       <c r="A19" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="20" t="s">
         <v>157</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -2083,7 +2088,7 @@
       <c r="A20" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B20" s="29">
+      <c r="B20" s="20">
         <v>1234</v>
       </c>
       <c r="C20" s="2" t="s">

</xml_diff>

<commit_message>
created new test for RFI forms; updated json files for account creation in SF; refactored Keyword Pattern in TestParametersController
</commit_message>
<xml_diff>
--- a/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/framework/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BPP\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BDD\framework\src\main\resources\data\bpp\keywords.metadata\metadata\UAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2346BEDB-0014-4663-BBA6-DBE77BCD6EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7B8E59-09BC-4C15-AD2E-3E37266E1944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23125" yWindow="-109" windowWidth="23451" windowHeight="14134" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="167">
   <si>
     <t>Tag</t>
   </si>
@@ -518,6 +518,12 @@
   </si>
   <si>
     <t>https://web-stage-bppdigital.bppuniversity.com/deactivateinstance</t>
+  </si>
+  <si>
+    <t>https://web-stage-bppdigital.bppuniversity.com/contact-bpp/request-information</t>
+  </si>
+  <si>
+    <t>BPPDIGITALRFILINK</t>
   </si>
 </sst>
 </file>
@@ -1519,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.55"/>
@@ -1826,6 +1832,17 @@
         <v>164</v>
       </c>
       <c r="C27" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1854,9 +1871,10 @@
     <hyperlink ref="B25" r:id="rId21" xr:uid="{490AA195-2BCD-46BA-A815-E8816723E15C}"/>
     <hyperlink ref="B26" r:id="rId22" xr:uid="{A2875131-586F-4E26-BAFD-7D53FBEA4B92}"/>
     <hyperlink ref="B27" r:id="rId23" xr:uid="{7528A15C-B863-45DE-89E2-AF2401542240}"/>
+    <hyperlink ref="B28" r:id="rId24" xr:uid="{BA1A336A-3C2E-447C-AF05-D5DA542DC306}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>